<commit_message>
- changed software architecture description
</commit_message>
<xml_diff>
--- a/03_Chefarchitekt/01_Methodik/Software-Architektur.xlsx
+++ b/03_Chefarchitekt/01_Methodik/Software-Architektur.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Außensicht</t>
   </si>
@@ -104,12 +104,6 @@
 subsys-B-default_impl</t>
   </si>
   <si>
-    <t>subsys-A-model</t>
-  </si>
-  <si>
-    <t>subsys-A-model-registry</t>
-  </si>
-  <si>
     <t>domain-data-model</t>
   </si>
   <si>
@@ -251,7 +245,16 @@
     <t>Subsubsystem (horizontal) ( fachlich motiviert?)</t>
   </si>
   <si>
-    <t>Ausprägung: Baumstruktur!</t>
+    <t>subsys-A-transient_data</t>
+  </si>
+  <si>
+    <t>subsys-A-transient_data-registry</t>
+  </si>
+  <si>
+    <t>Ausprägung einer Dimeniosn ist eine Baumstruktur!</t>
+  </si>
+  <si>
+    <t>extra Dimension??</t>
   </si>
 </sst>
 </file>
@@ -348,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -669,6 +672,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="1" tint="0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -678,7 +692,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -696,35 +710,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
@@ -735,88 +722,118 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1115,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1129,148 +1146,152 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="G1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="G2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="G2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:11">
+        <v>31</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="35"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>50</v>
+      <c r="D5" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H3:K3"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1280,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1291,64 +1312,64 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="38"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="50"/>
-      <c r="G1" s="51"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="52" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54" t="s">
+      <c r="E2" s="49"/>
+      <c r="F2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="30" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="56" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="57" t="s">
+      <c r="E3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>50</v>
+      <c r="F3" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32.25" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="41" t="s">
+      <c r="B4" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1362,9 +1383,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="61.5" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="27" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1376,29 +1397,29 @@
       <c r="F5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>35</v>
+      <c r="G5" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="45" t="s">
+      <c r="A6" s="44"/>
+      <c r="B6" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="42"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="45"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1406,53 +1427,53 @@
         <v>21</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="42"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
+      <c r="A8" s="44"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="46"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
+      <c r="D8" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A9" s="45"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="59"/>
       <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="15" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="24" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1477,7 +1498,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1490,48 +1511,48 @@
     <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="25" customFormat="1">
+    <row r="1" spans="1:8" s="16" customFormat="1">
       <c r="A1" s="1"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="55"/>
+      <c r="E1" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="26"/>
+      <c r="F1" s="55"/>
       <c r="G1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="31" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>44</v>
+      <c r="D2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -1540,163 +1561,163 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="31"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:8" ht="29.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+        <v>63</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" s="2"/>
@@ -1706,29 +1727,29 @@
       <c r="G14" s="2"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
+      <c r="B16" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C11:G11"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="C12:G12"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>